<commit_message>
Update scenario builder version
</commit_message>
<xml_diff>
--- a/scenario_builder_tool_input.xlsx
+++ b/scenario_builder_tool_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VincentLaguna\pypsa-eur-climact\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAEE125D-A4D1-44E2-86A7-F7B604A9F3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330C2394-40F0-4762-BC50-A5DBDFB4C023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Levers" sheetId="1" r:id="rId1"/>
@@ -800,7 +800,8 @@
     <t>Emissions from energy use  in agriculture</t>
   </si>
   <si>
-    <t>In refineries, energy carrier switch away from fossil fuels (from oil to gas, and to e-gas and biogas)</t>
+    <t xml:space="preserve">In refineries, energy carrier switch away from fossil fuels (from oil to gas, and to e-gas and biogas)
+</t>
   </si>
 </sst>
 </file>
@@ -876,11 +877,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1292,10 +1293,10 @@
   <dimension ref="A1:AE236"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E225" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3:E236"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1308,12 +1309,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" t="s">
         <v>237</v>
       </c>
@@ -20612,7 +20613,7 @@
       <c r="C206" t="s">
         <v>211</v>
       </c>
-      <c r="D206" s="7" t="s">
+      <c r="D206" s="6" t="s">
         <v>212</v>
       </c>
       <c r="E206">

</xml_diff>